<commit_message>
Pond depth measurment data
</commit_message>
<xml_diff>
--- a/Depth_Measurements/Ellens_Pond_Depth_Measurements.xlsx
+++ b/Depth_Measurements/Ellens_Pond_Depth_Measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kag326\Documents\Sediment_Mapping_DEC\Depth_Measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B7AF34-3D60-4561-B531-807ECD0C52B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CB069F-412E-44D5-A8C5-AF39790EF6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{EA217EAB-1D9D-4673-ACC6-F004AD8053C6}"/>
+    <workbookView xWindow="405" yWindow="750" windowWidth="21600" windowHeight="11385" xr2:uid="{EA217EAB-1D9D-4673-ACC6-F004AD8053C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>